<commit_message>
Dodan scenarij upotrebe aplikacije od strane uposlenika
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
+++ b/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
@@ -29,9 +29,6 @@
     <t>Kreiranje korisničkog računa</t>
   </si>
   <si>
-    <t>Korisnik  putem aplikacije podnosi zahtjev za otvaranje korisničkog računa</t>
-  </si>
-  <si>
     <t>Opis</t>
   </si>
   <si>
@@ -44,12 +41,6 @@
     <t>Korisnik mora imati pristup Internetu</t>
   </si>
   <si>
-    <t>Posljedice - uspješan završetak</t>
-  </si>
-  <si>
-    <t>Posljedice - neuspješan završetak</t>
-  </si>
-  <si>
     <t>Korisnik je kreirao svoj korisnički račun</t>
   </si>
   <si>
@@ -59,26 +50,35 @@
     <t>Primarni akteri</t>
   </si>
   <si>
-    <t>Korisnik, administrator</t>
-  </si>
-  <si>
     <t>Glavni tok</t>
   </si>
   <si>
-    <t>Korisnik podnosi zahtjev za formiranje korisničkog računa,  popuni odgovarajuće podatke, otvori korisnički račun</t>
-  </si>
-  <si>
     <t>Proširenja/Alternative</t>
   </si>
   <si>
     <t>Korisnik pogrešno unese podatke, sistem traži ponovni unos podataka</t>
+  </si>
+  <si>
+    <t>Posljedice – uspješan završetak</t>
+  </si>
+  <si>
+    <t>Posljedice – neuspješan završetak</t>
+  </si>
+  <si>
+    <t>Korisnik podnosi zahtjev za formiranje korisničkog računa, popuni odgovarajuće podatke, otvori korisnički račun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korisnik putem aplikacije podnosi zahtjev za otvaranje korisničkog računa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korisnik, administrator </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,22 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -113,17 +129,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyFont="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Style 1" xfId="1"/>
+    <cellStyle name="Style 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,69 +504,75 @@
     <col min="2" max="2" width="99.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dodan novi scenarij kreiranja korisničkog računa sa tokom događaja
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
+++ b/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Kreiranje korisničkog računa</t>
   </si>
@@ -72,13 +72,178 @@
   </si>
   <si>
     <t xml:space="preserve">Korisnik, administrator </t>
+  </si>
+  <si>
+    <t>Glavni tok događaja:</t>
+  </si>
+  <si>
+    <t>Korisnik</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pristupanje interfejsu aplikacije</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Podnošenje zahtjeva za otvaranje korisničkog računa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Popunjavanje osnovnih podataka</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Validacija zahtjeva</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dodjela sigurnosnog koda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Slanje povratne informacije</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +277,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -121,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -181,6 +353,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -189,7 +374,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -209,7 +394,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,19 +709,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="99.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -512,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -520,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -528,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -536,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -552,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -560,11 +777,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -574,7 +791,76 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
     </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="16"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Dodane ispravljene verzije za kreiranje korisnickog racuna
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
+++ b/UseCaseScenarij/Kreiranje korisničkog računa.xlsx
@@ -38,15 +38,9 @@
     <t>Preduvjeti</t>
   </si>
   <si>
-    <t>Korisnik mora imati pristup Internetu</t>
-  </si>
-  <si>
     <t>Korisnik je kreirao svoj korisnički račun</t>
   </si>
   <si>
-    <t>Korisnik dobiva obavijest da njegov račun nije kreiran i traži se ponovni unos podataka</t>
-  </si>
-  <si>
     <t>Primarni akteri</t>
   </si>
   <si>
@@ -56,16 +50,10 @@
     <t>Proširenja/Alternative</t>
   </si>
   <si>
-    <t>Korisnik pogrešno unese podatke, sistem traži ponovni unos podataka</t>
-  </si>
-  <si>
     <t>Posljedice – uspješan završetak</t>
   </si>
   <si>
     <t>Posljedice – neuspješan završetak</t>
-  </si>
-  <si>
-    <t>Korisnik podnosi zahtjev za formiranje korisničkog računa, popuni odgovarajuće podatke, otvori korisnički račun</t>
   </si>
   <si>
     <t xml:space="preserve">Korisnik putem aplikacije podnosi zahtjev za otvaranje korisničkog računa </t>
@@ -136,32 +124,6 @@
   </si>
   <si>
     <r>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Popunjavanje osnovnih podataka</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>4.</t>
     </r>
     <r>
@@ -187,56 +149,25 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dodjela sigurnosnog koda</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>6.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Slanje povratne informacije</t>
-    </r>
+    <t>Korisnik mora doći na Grasov šalter kako bi dao svoje podatke administratoru</t>
+  </si>
+  <si>
+    <t>Administrator pogrešno unese podatke, sistem traži ponovni unos podataka</t>
+  </si>
+  <si>
+    <t>3. Odlazak na Grasov šalter</t>
+  </si>
+  <si>
+    <t>5. Upis korisnikovih podataka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korisnik dobiva obavijest da njegov račun nije kreiran </t>
+  </si>
+  <si>
+    <t>Korisnik podnosi zahtjev za formiranje korisničkog računa, administrator popuni odgovarajuće podatke, otvori korisnički račun i dodjeli korisničko ime i password</t>
+  </si>
+  <si>
+    <t>6. Dodjela korisničkog imena i password-a</t>
   </si>
 </sst>
 </file>
@@ -412,6 +343,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -423,9 +357,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -711,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,55 +665,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -793,7 +724,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -807,51 +738,51 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" s="9"/>
     </row>
     <row r="17" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="17"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>

</xml_diff>